<commit_message>
updating testcase of adding 20 items into cart
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ALL_PAGES/END_TO_END/TC32_Verify_store_location.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ALL_PAGES/END_TO_END/TC32_Verify_store_location.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KamanProd\Input_files\Actual_testcases\Kaman\ALL_PAGES\END_TO_END\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KamanProd_ChangeBranch\Kaman_Production_Sanity\Input_files\Actual_testcases\Kaman\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6577A71-78BC-4EF6-A7E7-7A65C06B3A26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51586D5-79FE-4C1E-8AE7-A1181DA39FF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
   <si>
     <t>TestCase</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>$Registered_Password</t>
+  </si>
+  <si>
+    <t>MyaccountSection</t>
+  </si>
+  <si>
+    <t>Logout</t>
   </si>
 </sst>
 </file>
@@ -536,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A15" sqref="A15:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -746,6 +752,32 @@
       <c r="E14" s="3" t="s">
         <v>25</v>
       </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3"/>
+      <c r="B15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="3"/>
+      <c r="B16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -838,9 +870,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1041,19 +1076,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1078,9 +1109,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>